<commit_message>
Minor fix in PS table bit index
</commit_message>
<xml_diff>
--- a/development/L1Menu_Collisions2024_v1_1_0/PrescaleTable/L1Menu_Collisions2024_v1_1_0.xlsx
+++ b/development/L1Menu_Collisions2024_v1_1_0/PrescaleTable/L1Menu_Collisions2024_v1_1_0.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/caterinaaruta/Desktop/L1Menus/L1Menu_Collisions2024_v1_1_0/PStables_dev/PrescaleTable/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/caterinaaruta/Downloads/L1MenuRun3-master 25/development/L1Menu_Collisions2024_v1_1_0/PrescaleTable/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6E82C9A-2609-8840-A72C-D16A184B3B92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFC40B0F-CE5E-8546-B13A-C269DD82DD9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1622,8 +1622,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M391"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A325" workbookViewId="0">
-      <selection activeCell="C345" sqref="C345:M352"/>
+    <sheetView tabSelected="1" topLeftCell="A324" workbookViewId="0">
+      <selection activeCell="B343" sqref="B343"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -15459,7 +15459,7 @@
     </row>
     <row r="338" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A338">
-        <v>434</v>
+        <v>435</v>
       </c>
       <c r="B338" s="5" t="s">
         <v>397</v>
@@ -15500,7 +15500,7 @@
     </row>
     <row r="339" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A339">
-        <v>434</v>
+        <v>436</v>
       </c>
       <c r="B339" s="5" t="s">
         <v>398</v>

</xml_diff>

<commit_message>
PS change in DoubleEG11 seed
</commit_message>
<xml_diff>
--- a/development/L1Menu_Collisions2024_v1_1_0/PrescaleTable/L1Menu_Collisions2024_v1_1_0.xlsx
+++ b/development/L1Menu_Collisions2024_v1_1_0/PrescaleTable/L1Menu_Collisions2024_v1_1_0.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sonar\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/caterinaaruta/Downloads/L1MenuRun3_PSupdate/development/L1Menu_Collisions2024_v1_1_0/PrescaleTable/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60EC5665-B229-4696-A441-BA2540BE9BA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EB87973-1D51-4A42-AFE7-7B89CD09597D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1625,25 +1625,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N391"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K20" sqref="K20"/>
+    <sheetView tabSelected="1" topLeftCell="A173" workbookViewId="0">
+      <selection activeCell="O193" sqref="O193"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="60.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="60.1640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.6640625" customWidth="1"/>
     <col min="4" max="4" width="13" customWidth="1"/>
-    <col min="5" max="5" width="14.77734375" customWidth="1"/>
+    <col min="5" max="5" width="14.83203125" customWidth="1"/>
     <col min="6" max="6" width="14" customWidth="1"/>
     <col min="8" max="8" width="8" customWidth="1"/>
-    <col min="10" max="10" width="7.77734375" customWidth="1"/>
-    <col min="11" max="11" width="9.109375" customWidth="1"/>
+    <col min="10" max="10" width="7.83203125" customWidth="1"/>
+    <col min="11" max="11" width="9.1640625" customWidth="1"/>
     <col min="12" max="12" width="10.33203125" customWidth="1"/>
-    <col min="13" max="13" width="9.77734375" customWidth="1"/>
+    <col min="13" max="13" width="9.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="4" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" s="4" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1687,7 +1687,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>0</v>
       </c>
@@ -1731,7 +1731,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1</v>
       </c>
@@ -1775,7 +1775,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>2</v>
       </c>
@@ -1819,7 +1819,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>3</v>
       </c>
@@ -1863,7 +1863,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>4</v>
       </c>
@@ -1907,7 +1907,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>5</v>
       </c>
@@ -1951,7 +1951,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>6</v>
       </c>
@@ -1995,7 +1995,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>7</v>
       </c>
@@ -2039,7 +2039,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>8</v>
       </c>
@@ -2083,7 +2083,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>9</v>
       </c>
@@ -2127,7 +2127,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>10</v>
       </c>
@@ -2171,7 +2171,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>11</v>
       </c>
@@ -2215,7 +2215,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>12</v>
       </c>
@@ -2259,7 +2259,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>13</v>
       </c>
@@ -2303,7 +2303,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>14</v>
       </c>
@@ -2347,7 +2347,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>15</v>
       </c>
@@ -2391,7 +2391,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>16</v>
       </c>
@@ -2435,7 +2435,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>17</v>
       </c>
@@ -2479,7 +2479,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>18</v>
       </c>
@@ -2523,7 +2523,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>19</v>
       </c>
@@ -2567,7 +2567,7 @@
         <v>22000</v>
       </c>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>20</v>
       </c>
@@ -2611,7 +2611,7 @@
         <v>4400</v>
       </c>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>21</v>
       </c>
@@ -2655,7 +2655,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>22</v>
       </c>
@@ -2699,7 +2699,7 @@
         <v>2200</v>
       </c>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>23</v>
       </c>
@@ -2743,7 +2743,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>24</v>
       </c>
@@ -2787,7 +2787,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>25</v>
       </c>
@@ -2831,7 +2831,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>26</v>
       </c>
@@ -2875,7 +2875,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>27</v>
       </c>
@@ -2919,7 +2919,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>28</v>
       </c>
@@ -2963,7 +2963,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>29</v>
       </c>
@@ -3007,7 +3007,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>30</v>
       </c>
@@ -3051,7 +3051,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>31</v>
       </c>
@@ -3095,7 +3095,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>32</v>
       </c>
@@ -3139,7 +3139,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>33</v>
       </c>
@@ -3183,7 +3183,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>34</v>
       </c>
@@ -3227,7 +3227,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>35</v>
       </c>
@@ -3271,7 +3271,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>36</v>
       </c>
@@ -3315,7 +3315,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>37</v>
       </c>
@@ -3359,7 +3359,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>38</v>
       </c>
@@ -3403,7 +3403,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>39</v>
       </c>
@@ -3447,7 +3447,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>40</v>
       </c>
@@ -3491,7 +3491,7 @@
         <v>1500</v>
       </c>
     </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>41</v>
       </c>
@@ -3535,7 +3535,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>42</v>
       </c>
@@ -3579,7 +3579,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>43</v>
       </c>
@@ -3623,7 +3623,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>44</v>
       </c>
@@ -3667,7 +3667,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>45</v>
       </c>
@@ -3711,7 +3711,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>46</v>
       </c>
@@ -3755,7 +3755,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>47</v>
       </c>
@@ -3799,7 +3799,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>48</v>
       </c>
@@ -3843,7 +3843,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>49</v>
       </c>
@@ -3887,7 +3887,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A52">
         <v>50</v>
       </c>
@@ -3931,7 +3931,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A53">
         <v>51</v>
       </c>
@@ -3975,7 +3975,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A54">
         <v>52</v>
       </c>
@@ -4019,7 +4019,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A55">
         <v>53</v>
       </c>
@@ -4063,7 +4063,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A56">
         <v>54</v>
       </c>
@@ -4107,7 +4107,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A57">
         <v>55</v>
       </c>
@@ -4151,7 +4151,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A58">
         <v>56</v>
       </c>
@@ -4195,7 +4195,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A59">
         <v>57</v>
       </c>
@@ -4239,7 +4239,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A60">
         <v>58</v>
       </c>
@@ -4283,7 +4283,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A61">
         <v>59</v>
       </c>
@@ -4327,7 +4327,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A62">
         <v>60</v>
       </c>
@@ -4371,7 +4371,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="63" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A63">
         <v>61</v>
       </c>
@@ -4415,7 +4415,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="64" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A64">
         <v>62</v>
       </c>
@@ -4459,7 +4459,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="65" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A65">
         <v>63</v>
       </c>
@@ -4503,7 +4503,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="66" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A66">
         <v>64</v>
       </c>
@@ -4547,7 +4547,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A67">
         <v>65</v>
       </c>
@@ -4591,7 +4591,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="68" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A68">
         <v>66</v>
       </c>
@@ -4635,7 +4635,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="69" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A69">
         <v>67</v>
       </c>
@@ -4679,7 +4679,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A70">
         <v>68</v>
       </c>
@@ -4723,7 +4723,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A71">
         <v>69</v>
       </c>
@@ -4767,7 +4767,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="72" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A72">
         <v>70</v>
       </c>
@@ -4811,7 +4811,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="73" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A73">
         <v>71</v>
       </c>
@@ -4855,7 +4855,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A74">
         <v>72</v>
       </c>
@@ -4899,7 +4899,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="75" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A75">
         <v>73</v>
       </c>
@@ -4943,7 +4943,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A76">
         <v>74</v>
       </c>
@@ -4987,7 +4987,7 @@
         <v>700</v>
       </c>
     </row>
-    <row r="77" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A77">
         <v>75</v>
       </c>
@@ -5031,7 +5031,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A78">
         <v>76</v>
       </c>
@@ -5075,7 +5075,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="79" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A79">
         <v>77</v>
       </c>
@@ -5119,7 +5119,7 @@
         <v>800</v>
       </c>
     </row>
-    <row r="80" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A80">
         <v>78</v>
       </c>
@@ -5163,7 +5163,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="81" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A81">
         <v>79</v>
       </c>
@@ -5207,7 +5207,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="82" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A82">
         <v>80</v>
       </c>
@@ -5251,7 +5251,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="83" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A83">
         <v>81</v>
       </c>
@@ -5295,7 +5295,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="84" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A84">
         <v>82</v>
       </c>
@@ -5339,7 +5339,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A85">
         <v>83</v>
       </c>
@@ -5383,7 +5383,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A86">
         <v>84</v>
       </c>
@@ -5427,7 +5427,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A87">
         <v>85</v>
       </c>
@@ -5471,7 +5471,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A88">
         <v>86</v>
       </c>
@@ -5515,7 +5515,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A89">
         <v>87</v>
       </c>
@@ -5559,7 +5559,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="90" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A90">
         <v>88</v>
       </c>
@@ -5603,7 +5603,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="91" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A91">
         <v>89</v>
       </c>
@@ -5647,7 +5647,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="92" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A92">
         <v>90</v>
       </c>
@@ -5691,7 +5691,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="93" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A93">
         <v>91</v>
       </c>
@@ -5735,7 +5735,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="94" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A94">
         <v>92</v>
       </c>
@@ -5779,7 +5779,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="95" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A95">
         <v>93</v>
       </c>
@@ -5823,7 +5823,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="96" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A96">
         <v>94</v>
       </c>
@@ -5867,7 +5867,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="97" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A97">
         <v>95</v>
       </c>
@@ -5911,7 +5911,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A98">
         <v>96</v>
       </c>
@@ -5955,7 +5955,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="99" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A99">
         <v>97</v>
       </c>
@@ -5999,7 +5999,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="100" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A100">
         <v>98</v>
       </c>
@@ -6043,7 +6043,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="101" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A101">
         <v>99</v>
       </c>
@@ -6087,7 +6087,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="102" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A102">
         <v>100</v>
       </c>
@@ -6131,7 +6131,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="103" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A103">
         <v>101</v>
       </c>
@@ -6175,7 +6175,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="104" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A104">
         <v>102</v>
       </c>
@@ -6219,7 +6219,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="105" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A105">
         <v>103</v>
       </c>
@@ -6263,7 +6263,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="106" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A106">
         <v>104</v>
       </c>
@@ -6307,7 +6307,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="107" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A107">
         <v>105</v>
       </c>
@@ -6351,7 +6351,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="108" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A108">
         <v>106</v>
       </c>
@@ -6395,7 +6395,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="109" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A109">
         <v>107</v>
       </c>
@@ -6439,7 +6439,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="110" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A110">
         <v>108</v>
       </c>
@@ -6483,7 +6483,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="111" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A111">
         <v>109</v>
       </c>
@@ -6527,7 +6527,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="112" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A112">
         <v>110</v>
       </c>
@@ -6571,7 +6571,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="113" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A113">
         <v>111</v>
       </c>
@@ -6615,7 +6615,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="114" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A114">
         <v>112</v>
       </c>
@@ -6659,7 +6659,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="115" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A115">
         <v>113</v>
       </c>
@@ -6703,7 +6703,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="116" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A116">
         <v>114</v>
       </c>
@@ -6747,7 +6747,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="117" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A117">
         <v>115</v>
       </c>
@@ -6791,7 +6791,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="118" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A118">
         <v>116</v>
       </c>
@@ -6835,7 +6835,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="119" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A119">
         <v>117</v>
       </c>
@@ -6879,7 +6879,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="120" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A120">
         <v>119</v>
       </c>
@@ -6923,7 +6923,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="121" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A121">
         <v>120</v>
       </c>
@@ -6967,7 +6967,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="122" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A122">
         <v>122</v>
       </c>
@@ -7011,7 +7011,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="123" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A123">
         <v>123</v>
       </c>
@@ -7055,7 +7055,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="124" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A124">
         <v>124</v>
       </c>
@@ -7099,7 +7099,7 @@
         <v>11000</v>
       </c>
     </row>
-    <row r="125" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A125">
         <v>125</v>
       </c>
@@ -7143,7 +7143,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="126" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A126">
         <v>126</v>
       </c>
@@ -7187,7 +7187,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="127" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A127">
         <v>127</v>
       </c>
@@ -7231,7 +7231,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="128" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A128">
         <v>128</v>
       </c>
@@ -7275,7 +7275,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="129" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A129">
         <v>129</v>
       </c>
@@ -7319,7 +7319,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="130" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A130">
         <v>130</v>
       </c>
@@ -7363,7 +7363,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="131" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A131">
         <v>131</v>
       </c>
@@ -7407,7 +7407,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="132" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A132">
         <v>132</v>
       </c>
@@ -7451,7 +7451,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="133" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A133">
         <v>133</v>
       </c>
@@ -7495,7 +7495,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="134" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A134">
         <v>134</v>
       </c>
@@ -7539,7 +7539,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="135" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A135">
         <v>135</v>
       </c>
@@ -7583,7 +7583,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="136" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A136">
         <v>136</v>
       </c>
@@ -7627,7 +7627,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="137" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A137">
         <v>137</v>
       </c>
@@ -7671,7 +7671,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="138" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A138">
         <v>138</v>
       </c>
@@ -7715,7 +7715,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="139" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A139">
         <v>139</v>
       </c>
@@ -7759,7 +7759,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="140" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A140">
         <v>140</v>
       </c>
@@ -7803,7 +7803,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="141" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A141">
         <v>141</v>
       </c>
@@ -7847,7 +7847,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="142" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A142">
         <v>144</v>
       </c>
@@ -7891,7 +7891,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="143" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A143">
         <v>147</v>
       </c>
@@ -7935,7 +7935,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="144" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A144">
         <v>148</v>
       </c>
@@ -7979,7 +7979,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="145" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A145">
         <v>149</v>
       </c>
@@ -8023,7 +8023,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="146" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A146">
         <v>150</v>
       </c>
@@ -8067,7 +8067,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="147" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A147">
         <v>151</v>
       </c>
@@ -8111,7 +8111,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="148" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A148">
         <v>152</v>
       </c>
@@ -8155,7 +8155,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="149" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A149">
         <v>153</v>
       </c>
@@ -8199,7 +8199,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="150" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A150">
         <v>154</v>
       </c>
@@ -8243,7 +8243,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="151" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A151">
         <v>156</v>
       </c>
@@ -8287,7 +8287,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="152" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A152">
         <v>159</v>
       </c>
@@ -8331,7 +8331,7 @@
         <v>44000</v>
       </c>
     </row>
-    <row r="153" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A153">
         <v>160</v>
       </c>
@@ -8375,7 +8375,7 @@
         <v>9000</v>
       </c>
     </row>
-    <row r="154" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A154">
         <v>161</v>
       </c>
@@ -8419,7 +8419,7 @@
         <v>1550</v>
       </c>
     </row>
-    <row r="155" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A155">
         <v>162</v>
       </c>
@@ -8463,7 +8463,7 @@
         <v>780</v>
       </c>
     </row>
-    <row r="156" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A156">
         <v>163</v>
       </c>
@@ -8507,7 +8507,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="157" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A157">
         <v>164</v>
       </c>
@@ -8551,7 +8551,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="158" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A158">
         <v>165</v>
       </c>
@@ -8595,7 +8595,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="159" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A159">
         <v>166</v>
       </c>
@@ -8639,7 +8639,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="160" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A160">
         <v>167</v>
       </c>
@@ -8683,7 +8683,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="161" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A161">
         <v>168</v>
       </c>
@@ -8727,7 +8727,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="162" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A162">
         <v>169</v>
       </c>
@@ -8771,7 +8771,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="163" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A163">
         <v>170</v>
       </c>
@@ -8815,7 +8815,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="164" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A164">
         <v>171</v>
       </c>
@@ -8859,7 +8859,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="165" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A165">
         <v>172</v>
       </c>
@@ -8903,7 +8903,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="166" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A166">
         <v>173</v>
       </c>
@@ -8947,7 +8947,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="167" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A167">
         <v>174</v>
       </c>
@@ -8991,7 +8991,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="168" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A168">
         <v>175</v>
       </c>
@@ -9035,7 +9035,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="169" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A169">
         <v>176</v>
       </c>
@@ -9079,7 +9079,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="170" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A170">
         <v>177</v>
       </c>
@@ -9123,7 +9123,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="171" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A171">
         <v>178</v>
       </c>
@@ -9167,7 +9167,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="172" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A172">
         <v>179</v>
       </c>
@@ -9211,7 +9211,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="173" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A173">
         <v>180</v>
       </c>
@@ -9255,7 +9255,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="174" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A174">
         <v>181</v>
       </c>
@@ -9299,7 +9299,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="175" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A175">
         <v>182</v>
       </c>
@@ -9343,7 +9343,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="176" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A176">
         <v>183</v>
       </c>
@@ -9387,7 +9387,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="177" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A177">
         <v>185</v>
       </c>
@@ -9431,7 +9431,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="178" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A178">
         <v>186</v>
       </c>
@@ -9475,7 +9475,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="179" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A179">
         <v>188</v>
       </c>
@@ -9519,7 +9519,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="180" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A180">
         <v>189</v>
       </c>
@@ -9563,7 +9563,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="181" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A181">
         <v>190</v>
       </c>
@@ -9607,7 +9607,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="182" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A182">
         <v>191</v>
       </c>
@@ -9651,7 +9651,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="183" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A183">
         <v>192</v>
       </c>
@@ -9695,7 +9695,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="184" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A184">
         <v>193</v>
       </c>
@@ -9739,7 +9739,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="185" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A185">
         <v>194</v>
       </c>
@@ -9783,7 +9783,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="186" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A186">
         <v>195</v>
       </c>
@@ -9827,7 +9827,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="187" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A187">
         <v>196</v>
       </c>
@@ -9871,7 +9871,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="188" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A188">
         <v>197</v>
       </c>
@@ -9915,7 +9915,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="189" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A189">
         <v>198</v>
       </c>
@@ -9959,7 +9959,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="190" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A190">
         <v>199</v>
       </c>
@@ -10003,7 +10003,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="191" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A191">
         <v>200</v>
       </c>
@@ -10047,7 +10047,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="192" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A192">
         <v>201</v>
       </c>
@@ -10091,7 +10091,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="193" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A193">
         <v>214</v>
       </c>
@@ -10102,40 +10102,40 @@
         <v>0</v>
       </c>
       <c r="D193" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E193" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F193" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G193" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H193" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I193" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J193" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K193" s="1">
         <v>0</v>
       </c>
       <c r="L193" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M193" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N193" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="194" spans="1:14" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="194" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A194">
         <v>215</v>
       </c>
@@ -10179,7 +10179,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="195" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A195">
         <v>216</v>
       </c>
@@ -10223,7 +10223,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="196" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A196">
         <v>217</v>
       </c>
@@ -10267,7 +10267,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="197" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A197">
         <v>218</v>
       </c>
@@ -10311,7 +10311,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="198" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A198">
         <v>219</v>
       </c>
@@ -10355,7 +10355,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="199" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="199" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A199">
         <v>220</v>
       </c>
@@ -10399,7 +10399,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="200" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="200" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A200">
         <v>223</v>
       </c>
@@ -10443,7 +10443,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="201" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="201" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A201">
         <v>224</v>
       </c>
@@ -10487,7 +10487,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="202" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="202" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A202">
         <v>225</v>
       </c>
@@ -10531,7 +10531,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="203" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="203" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A203">
         <v>226</v>
       </c>
@@ -10575,7 +10575,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="204" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="204" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A204">
         <v>227</v>
       </c>
@@ -10619,7 +10619,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="205" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="205" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A205">
         <v>228</v>
       </c>
@@ -10663,7 +10663,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="206" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="206" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A206">
         <v>229</v>
       </c>
@@ -10707,7 +10707,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="207" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="207" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A207">
         <v>230</v>
       </c>
@@ -10751,7 +10751,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="208" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="208" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A208">
         <v>231</v>
       </c>
@@ -10795,7 +10795,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="209" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="209" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A209">
         <v>234</v>
       </c>
@@ -10839,7 +10839,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="210" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="210" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A210">
         <v>235</v>
       </c>
@@ -10883,7 +10883,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="211" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="211" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A211">
         <v>238</v>
       </c>
@@ -10927,7 +10927,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="212" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="212" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A212">
         <v>239</v>
       </c>
@@ -10971,7 +10971,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="213" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="213" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A213">
         <v>240</v>
       </c>
@@ -11015,7 +11015,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="214" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="214" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A214">
         <v>241</v>
       </c>
@@ -11059,7 +11059,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="215" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="215" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A215">
         <v>242</v>
       </c>
@@ -11103,7 +11103,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="216" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="216" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A216">
         <v>243</v>
       </c>
@@ -11147,7 +11147,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="217" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="217" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A217">
         <v>244</v>
       </c>
@@ -11191,7 +11191,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="218" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="218" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A218">
         <v>245</v>
       </c>
@@ -11235,7 +11235,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="219" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="219" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A219">
         <v>248</v>
       </c>
@@ -11279,7 +11279,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="220" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="220" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A220">
         <v>249</v>
       </c>
@@ -11323,7 +11323,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="221" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="221" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A221">
         <v>250</v>
       </c>
@@ -11367,7 +11367,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="222" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="222" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A222">
         <v>257</v>
       </c>
@@ -11411,7 +11411,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="223" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="223" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A223">
         <v>258</v>
       </c>
@@ -11455,7 +11455,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="224" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="224" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A224">
         <v>259</v>
       </c>
@@ -11499,7 +11499,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="225" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="225" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A225">
         <v>263</v>
       </c>
@@ -11543,7 +11543,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="226" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="226" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A226">
         <v>264</v>
       </c>
@@ -11587,7 +11587,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="227" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="227" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A227">
         <v>266</v>
       </c>
@@ -11631,7 +11631,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="228" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="228" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A228">
         <v>267</v>
       </c>
@@ -11675,7 +11675,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="229" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="229" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A229">
         <v>268</v>
       </c>
@@ -11719,7 +11719,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="230" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="230" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A230">
         <v>269</v>
       </c>
@@ -11763,7 +11763,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="231" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="231" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A231">
         <v>270</v>
       </c>
@@ -11807,7 +11807,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="232" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="232" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A232">
         <v>271</v>
       </c>
@@ -11851,7 +11851,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="233" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="233" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A233">
         <v>272</v>
       </c>
@@ -11895,7 +11895,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="234" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="234" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A234">
         <v>278</v>
       </c>
@@ -11939,7 +11939,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="235" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="235" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A235">
         <v>279</v>
       </c>
@@ -11983,7 +11983,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="236" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="236" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A236">
         <v>280</v>
       </c>
@@ -12027,7 +12027,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="237" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="237" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A237">
         <v>281</v>
       </c>
@@ -12071,7 +12071,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="238" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="238" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A238">
         <v>282</v>
       </c>
@@ -12115,7 +12115,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="239" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="239" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A239">
         <v>283</v>
       </c>
@@ -12159,7 +12159,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="240" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="240" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A240">
         <v>284</v>
       </c>
@@ -12203,7 +12203,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="241" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="241" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A241">
         <v>286</v>
       </c>
@@ -12247,7 +12247,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="242" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="242" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A242">
         <v>287</v>
       </c>
@@ -12291,7 +12291,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="243" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="243" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A243">
         <v>288</v>
       </c>
@@ -12335,7 +12335,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="244" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="244" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A244">
         <v>290</v>
       </c>
@@ -12379,7 +12379,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="245" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="245" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A245">
         <v>291</v>
       </c>
@@ -12423,7 +12423,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="246" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="246" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A246">
         <v>298</v>
       </c>
@@ -12467,7 +12467,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="247" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="247" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A247">
         <v>305</v>
       </c>
@@ -12511,7 +12511,7 @@
         <v>64000</v>
       </c>
     </row>
-    <row r="248" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="248" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A248">
         <v>306</v>
       </c>
@@ -12555,7 +12555,7 @@
         <v>17000</v>
       </c>
     </row>
-    <row r="249" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="249" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A249">
         <v>307</v>
       </c>
@@ -12599,7 +12599,7 @@
         <v>1500</v>
       </c>
     </row>
-    <row r="250" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="250" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A250">
         <v>308</v>
       </c>
@@ -12643,7 +12643,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="251" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="251" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A251">
         <v>309</v>
       </c>
@@ -12687,7 +12687,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="252" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="252" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A252">
         <v>310</v>
       </c>
@@ -12731,7 +12731,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="253" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="253" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A253">
         <v>311</v>
       </c>
@@ -12775,7 +12775,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="254" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="254" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A254">
         <v>312</v>
       </c>
@@ -12819,7 +12819,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="255" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="255" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A255">
         <v>314</v>
       </c>
@@ -12863,7 +12863,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="256" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="256" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A256">
         <v>315</v>
       </c>
@@ -12907,7 +12907,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="257" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="257" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A257">
         <v>316</v>
       </c>
@@ -12951,7 +12951,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="258" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="258" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A258">
         <v>317</v>
       </c>
@@ -12995,7 +12995,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="259" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="259" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A259">
         <v>318</v>
       </c>
@@ -13039,7 +13039,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="260" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="260" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A260">
         <v>320</v>
       </c>
@@ -13083,7 +13083,7 @@
         <v>28327</v>
       </c>
     </row>
-    <row r="261" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="261" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A261">
         <v>321</v>
       </c>
@@ -13127,7 +13127,7 @@
         <v>1820</v>
       </c>
     </row>
-    <row r="262" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="262" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A262">
         <v>322</v>
       </c>
@@ -13171,7 +13171,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="263" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="263" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A263">
         <v>323</v>
       </c>
@@ -13215,7 +13215,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="264" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="264" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A264">
         <v>324</v>
       </c>
@@ -13259,7 +13259,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="265" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="265" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A265">
         <v>327</v>
       </c>
@@ -13303,7 +13303,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="266" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="266" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A266">
         <v>328</v>
       </c>
@@ -13347,7 +13347,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="267" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="267" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A267">
         <v>329</v>
       </c>
@@ -13391,7 +13391,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="268" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="268" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A268">
         <v>330</v>
       </c>
@@ -13435,7 +13435,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="269" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="269" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A269">
         <v>334</v>
       </c>
@@ -13479,7 +13479,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="270" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="270" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A270">
         <v>335</v>
       </c>
@@ -13523,7 +13523,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="271" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="271" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A271">
         <v>336</v>
       </c>
@@ -13567,7 +13567,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="272" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="272" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A272">
         <v>337</v>
       </c>
@@ -13611,7 +13611,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="273" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="273" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A273">
         <v>340</v>
       </c>
@@ -13655,7 +13655,7 @@
         <v>8400</v>
       </c>
     </row>
-    <row r="274" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="274" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A274">
         <v>341</v>
       </c>
@@ -13699,7 +13699,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="275" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="275" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A275">
         <v>342</v>
       </c>
@@ -13743,7 +13743,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="276" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="276" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A276">
         <v>343</v>
       </c>
@@ -13787,7 +13787,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="277" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="277" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A277">
         <v>345</v>
       </c>
@@ -13831,7 +13831,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="278" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="278" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A278">
         <v>346</v>
       </c>
@@ -13875,7 +13875,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="279" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="279" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A279">
         <v>347</v>
       </c>
@@ -13919,7 +13919,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="280" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="280" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A280">
         <v>348</v>
       </c>
@@ -13963,7 +13963,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="281" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="281" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A281">
         <v>349</v>
       </c>
@@ -14007,7 +14007,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="282" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="282" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A282">
         <v>350</v>
       </c>
@@ -14051,7 +14051,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="283" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="283" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A283">
         <v>357</v>
       </c>
@@ -14095,7 +14095,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="284" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="284" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A284">
         <v>358</v>
       </c>
@@ -14139,7 +14139,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="285" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="285" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A285">
         <v>362</v>
       </c>
@@ -14183,7 +14183,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="286" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="286" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A286">
         <v>363</v>
       </c>
@@ -14227,7 +14227,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="287" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="287" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A287">
         <v>364</v>
       </c>
@@ -14271,7 +14271,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="288" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="288" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A288">
         <v>365</v>
       </c>
@@ -14315,7 +14315,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="289" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="289" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A289">
         <v>366</v>
       </c>
@@ -14359,7 +14359,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="290" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="290" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A290">
         <v>367</v>
       </c>
@@ -14403,7 +14403,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="291" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="291" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A291">
         <v>368</v>
       </c>
@@ -14447,7 +14447,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="292" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="292" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A292">
         <v>369</v>
       </c>
@@ -14491,7 +14491,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="293" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="293" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A293">
         <v>370</v>
       </c>
@@ -14535,7 +14535,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="294" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="294" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A294">
         <v>371</v>
       </c>
@@ -14579,7 +14579,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="295" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="295" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A295">
         <v>383</v>
       </c>
@@ -14623,7 +14623,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="296" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="296" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A296">
         <v>384</v>
       </c>
@@ -14667,7 +14667,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="297" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="297" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A297">
         <v>385</v>
       </c>
@@ -14711,7 +14711,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="298" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="298" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A298">
         <v>386</v>
       </c>
@@ -14755,7 +14755,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="299" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="299" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A299">
         <v>389</v>
       </c>
@@ -14799,7 +14799,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="300" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="300" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A300">
         <v>390</v>
       </c>
@@ -14843,7 +14843,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="301" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="301" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A301">
         <v>391</v>
       </c>
@@ -14887,7 +14887,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="302" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="302" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A302">
         <v>392</v>
       </c>
@@ -14931,7 +14931,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="303" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="303" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A303">
         <v>393</v>
       </c>
@@ -14975,7 +14975,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="304" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="304" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A304">
         <v>394</v>
       </c>
@@ -15019,7 +15019,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="305" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="305" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A305">
         <v>395</v>
       </c>
@@ -15063,7 +15063,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="306" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="306" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A306">
         <v>396</v>
       </c>
@@ -15107,7 +15107,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="307" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="307" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A307">
         <v>397</v>
       </c>
@@ -15151,7 +15151,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="308" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="308" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A308">
         <v>398</v>
       </c>
@@ -15195,7 +15195,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="309" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="309" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A309">
         <v>402</v>
       </c>
@@ -15239,7 +15239,7 @@
         <v>11400</v>
       </c>
     </row>
-    <row r="310" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="310" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A310">
         <v>403</v>
       </c>
@@ -15283,7 +15283,7 @@
         <v>4100</v>
       </c>
     </row>
-    <row r="311" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="311" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A311">
         <v>404</v>
       </c>
@@ -15327,7 +15327,7 @@
         <v>1600</v>
       </c>
     </row>
-    <row r="312" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="312" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A312">
         <v>405</v>
       </c>
@@ -15371,7 +15371,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="313" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="313" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A313">
         <v>406</v>
       </c>
@@ -15415,7 +15415,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="314" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="314" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A314">
         <v>407</v>
       </c>
@@ -15459,7 +15459,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="315" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="315" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A315">
         <v>408</v>
       </c>
@@ -15503,7 +15503,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="316" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="316" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A316">
         <v>409</v>
       </c>
@@ -15547,7 +15547,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="317" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="317" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A317">
         <v>410</v>
       </c>
@@ -15591,7 +15591,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="318" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="318" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A318">
         <v>412</v>
       </c>
@@ -15635,7 +15635,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="319" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="319" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A319">
         <v>416</v>
       </c>
@@ -15679,7 +15679,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="320" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="320" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A320">
         <v>417</v>
       </c>
@@ -15723,7 +15723,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="321" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="321" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A321">
         <v>418</v>
       </c>
@@ -15767,7 +15767,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="322" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="322" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A322">
         <v>419</v>
       </c>
@@ -15811,7 +15811,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="323" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="323" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A323">
         <v>420</v>
       </c>
@@ -15855,7 +15855,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="324" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="324" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A324">
         <v>421</v>
       </c>
@@ -15899,7 +15899,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="325" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="325" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A325">
         <v>422</v>
       </c>
@@ -15943,7 +15943,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="326" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="326" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A326">
         <v>423</v>
       </c>
@@ -15987,7 +15987,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="327" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="327" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A327">
         <v>424</v>
       </c>
@@ -16031,7 +16031,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="328" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="328" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A328">
         <v>425</v>
       </c>
@@ -16075,7 +16075,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="329" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="329" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A329">
         <v>426</v>
       </c>
@@ -16119,7 +16119,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="330" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="330" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A330">
         <v>427</v>
       </c>
@@ -16163,7 +16163,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="331" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="331" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A331">
         <v>428</v>
       </c>
@@ -16207,7 +16207,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="332" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="332" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A332">
         <v>429</v>
       </c>
@@ -16251,7 +16251,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="333" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="333" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A333">
         <v>430</v>
       </c>
@@ -16295,7 +16295,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="334" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="334" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A334">
         <v>431</v>
       </c>
@@ -16339,7 +16339,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="335" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="335" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A335">
         <v>432</v>
       </c>
@@ -16383,7 +16383,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="336" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="336" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A336">
         <v>433</v>
       </c>
@@ -16427,7 +16427,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="337" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="337" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A337">
         <v>434</v>
       </c>
@@ -16471,7 +16471,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="338" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="338" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A338">
         <v>435</v>
       </c>
@@ -16515,7 +16515,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="339" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="339" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A339">
         <v>436</v>
       </c>
@@ -16559,7 +16559,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="340" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="340" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A340">
         <v>438</v>
       </c>
@@ -16603,7 +16603,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="341" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="341" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A341">
         <v>439</v>
       </c>
@@ -16647,7 +16647,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="342" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="342" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A342">
         <v>440</v>
       </c>
@@ -16691,7 +16691,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="343" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="343" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A343">
         <v>441</v>
       </c>
@@ -16735,7 +16735,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="344" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="344" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A344">
         <v>442</v>
       </c>
@@ -16779,7 +16779,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="345" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="345" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A345">
         <v>446</v>
       </c>
@@ -16823,7 +16823,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="346" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="346" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A346">
         <v>447</v>
       </c>
@@ -16867,7 +16867,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="347" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="347" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A347">
         <v>448</v>
       </c>
@@ -16911,7 +16911,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="348" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="348" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A348">
         <v>451</v>
       </c>
@@ -16955,7 +16955,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="349" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="349" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A349">
         <v>452</v>
       </c>
@@ -16999,7 +16999,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="350" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="350" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A350">
         <v>453</v>
       </c>
@@ -17043,7 +17043,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="351" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="351" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A351">
         <v>454</v>
       </c>
@@ -17087,7 +17087,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="352" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="352" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A352">
         <v>458</v>
       </c>
@@ -17131,7 +17131,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="353" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="353" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A353">
         <v>459</v>
       </c>
@@ -17175,7 +17175,7 @@
         <v>17581</v>
       </c>
     </row>
-    <row r="354" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="354" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A354">
         <v>460</v>
       </c>
@@ -17219,7 +17219,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="355" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="355" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A355">
         <v>461</v>
       </c>
@@ -17263,7 +17263,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="356" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="356" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A356">
         <v>462</v>
       </c>
@@ -17307,7 +17307,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="357" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="357" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A357">
         <v>463</v>
       </c>
@@ -17351,7 +17351,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="358" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="358" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A358">
         <v>464</v>
       </c>
@@ -17395,7 +17395,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="359" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="359" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A359">
         <v>465</v>
       </c>
@@ -17439,7 +17439,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="360" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="360" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A360">
         <v>466</v>
       </c>
@@ -17483,7 +17483,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="361" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="361" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A361">
         <v>467</v>
       </c>
@@ -17527,7 +17527,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="362" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="362" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A362">
         <v>468</v>
       </c>
@@ -17571,7 +17571,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="363" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="363" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A363">
         <v>469</v>
       </c>
@@ -17615,7 +17615,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="364" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="364" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A364">
         <v>471</v>
       </c>
@@ -17659,7 +17659,7 @@
         <v>2239</v>
       </c>
     </row>
-    <row r="365" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="365" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A365">
         <v>472</v>
       </c>
@@ -17703,7 +17703,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="366" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="366" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A366">
         <v>473</v>
       </c>
@@ -17747,7 +17747,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="367" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="367" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A367">
         <v>474</v>
       </c>
@@ -17791,7 +17791,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="368" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="368" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A368">
         <v>475</v>
       </c>
@@ -17835,7 +17835,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="369" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="369" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A369">
         <v>476</v>
       </c>
@@ -17879,7 +17879,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="370" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="370" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A370">
         <v>477</v>
       </c>
@@ -17923,7 +17923,7 @@
         <v>56237</v>
       </c>
     </row>
-    <row r="371" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="371" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A371">
         <v>478</v>
       </c>
@@ -17967,7 +17967,7 @@
         <v>56237</v>
       </c>
     </row>
-    <row r="372" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="372" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A372">
         <v>479</v>
       </c>
@@ -18011,7 +18011,7 @@
         <v>59051</v>
       </c>
     </row>
-    <row r="373" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="373" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A373">
         <v>480</v>
       </c>
@@ -18055,7 +18055,7 @@
         <v>563</v>
       </c>
     </row>
-    <row r="374" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="374" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A374">
         <v>482</v>
       </c>
@@ -18099,7 +18099,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="375" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="375" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A375">
         <v>483</v>
       </c>
@@ -18143,7 +18143,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="376" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="376" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A376">
         <v>484</v>
       </c>
@@ -18187,7 +18187,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="377" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="377" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A377">
         <v>485</v>
       </c>
@@ -18231,7 +18231,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="378" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="378" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A378">
         <v>486</v>
       </c>
@@ -18275,7 +18275,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="379" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="379" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A379">
         <v>487</v>
       </c>
@@ -18319,7 +18319,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="380" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="380" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A380">
         <v>488</v>
       </c>
@@ -18363,7 +18363,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="381" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="381" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A381">
         <v>489</v>
       </c>
@@ -18407,7 +18407,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="382" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="382" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A382">
         <v>490</v>
       </c>
@@ -18451,7 +18451,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="383" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="383" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A383">
         <v>491</v>
       </c>
@@ -18495,7 +18495,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="384" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="384" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A384">
         <v>492</v>
       </c>
@@ -18539,7 +18539,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="385" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="385" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A385">
         <v>494</v>
       </c>
@@ -18583,7 +18583,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="386" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="386" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A386">
         <v>500</v>
       </c>
@@ -18627,7 +18627,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="387" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="387" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A387">
         <v>501</v>
       </c>
@@ -18671,7 +18671,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="388" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="388" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A388">
         <v>503</v>
       </c>
@@ -18715,7 +18715,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="389" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="389" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A389">
         <v>504</v>
       </c>
@@ -18759,7 +18759,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="390" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="390" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A390">
         <v>505</v>
       </c>
@@ -18803,7 +18803,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="391" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="391" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A391">
         <v>506</v>
       </c>

</xml_diff>